<commit_message>
update README, update test data and scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -42,15 +42,6 @@
     <t>TC2</t>
   </si>
   <si>
-    <t>abc@xyz.com</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -67,27 +58,6 @@
   </si>
   <si>
     <t>message</t>
-  </si>
-  <si>
-    <t>Customer service</t>
-  </si>
-  <si>
-    <t>abc@123.com</t>
-  </si>
-  <si>
-    <t>Testmessage1</t>
-  </si>
-  <si>
-    <t>Testmessage2</t>
-  </si>
-  <si>
-    <t>abc@234.com</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>bcd234</t>
   </si>
 </sst>
 </file>
@@ -473,7 +443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -491,90 +463,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="F2" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>